<commit_message>
Further updates to figure
</commit_message>
<xml_diff>
--- a/files/instrument_calibrations.xlsx
+++ b/files/instrument_calibrations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justin.belluz\Documents\R\chl_qc\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26F2B7F-5A02-4E9D-ADE7-396623C5723B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403D43CB-B0E0-4E5D-BF98-1E33DCC709FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{7EE5C623-4CD7-4802-A0BC-AFE8F0D74600}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>lab</t>
+  </si>
+  <si>
+    <t>Hakai</t>
+  </si>
+  <si>
+    <t>DFO</t>
   </si>
 </sst>
 </file>
@@ -518,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2529F593-B02A-4ABF-8304-BC32445D0581}">
-  <dimension ref="A1:X153"/>
+  <dimension ref="A1:Y153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M67" sqref="M67:M78"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="X124" sqref="X124:X153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,7 +539,7 @@
     <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,10 +610,13 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>42082</v>
       </c>
@@ -671,8 +683,11 @@
       <c r="W2">
         <v>8.4978342696666667E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>42082</v>
       </c>
@@ -739,8 +754,11 @@
       <c r="W3">
         <v>0.19161324101838295</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>42082</v>
       </c>
@@ -807,8 +825,11 @@
       <c r="W4">
         <v>2.5895224898897472E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>42082</v>
       </c>
@@ -875,8 +896,11 @@
       <c r="W5">
         <v>0.1242215079701067</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>42082</v>
       </c>
@@ -943,8 +967,11 @@
       <c r="W6">
         <v>9.5641295970602641E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>42082</v>
       </c>
@@ -1011,8 +1038,11 @@
       <c r="W7">
         <v>5.3535131415384761E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>42082</v>
       </c>
@@ -1079,8 +1109,11 @@
       <c r="W8">
         <v>6.270636809331441E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>42082</v>
       </c>
@@ -1147,8 +1180,11 @@
       <c r="W9">
         <v>5.8629350797212043E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>42082</v>
       </c>
@@ -1215,8 +1251,11 @@
       <c r="W10">
         <v>6.2751925724537846E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>42082</v>
       </c>
@@ -1283,8 +1322,11 @@
       <c r="W11">
         <v>6.4512595895306777E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>42082</v>
       </c>
@@ -1351,8 +1393,11 @@
       <c r="W12">
         <v>1.5985200879273711E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>42082</v>
       </c>
@@ -1419,8 +1464,11 @@
       <c r="W13">
         <v>9.89731616941621E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>42082</v>
       </c>
@@ -1487,8 +1535,11 @@
       <c r="W14">
         <v>4.6924868813578583E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>42222</v>
       </c>
@@ -1555,8 +1606,11 @@
       <c r="W15">
         <v>0.11962199954152029</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>42222</v>
       </c>
@@ -1623,8 +1677,11 @@
       <c r="W16">
         <v>0.1378650905205</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>42222</v>
       </c>
@@ -1691,8 +1748,11 @@
       <c r="W17">
         <v>2.4966259105380691E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>42222</v>
       </c>
@@ -1759,8 +1819,11 @@
       <c r="W18">
         <v>3.9157803950622724E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>42222</v>
       </c>
@@ -1815,8 +1878,11 @@
       <c r="U19">
         <v>4.5600000000000005</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>42222</v>
       </c>
@@ -1883,8 +1949,11 @@
       <c r="W20">
         <v>4.5668035751513486E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>42222</v>
       </c>
@@ -1951,8 +2020,11 @@
       <c r="W21">
         <v>2.3788974042137877E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>42222</v>
       </c>
@@ -2019,8 +2091,11 @@
       <c r="W22">
         <v>2.7525002317725429E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>42222</v>
       </c>
@@ -2087,8 +2162,11 @@
       <c r="W23">
         <v>6.6723805867557454E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>42222</v>
       </c>
@@ -2155,8 +2233,11 @@
       <c r="W24">
         <v>8.3916784554501061E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>42222</v>
       </c>
@@ -2223,8 +2304,11 @@
       <c r="W25">
         <v>3.5514194848709642E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>42222</v>
       </c>
@@ -2291,8 +2375,11 @@
       <c r="W26">
         <v>4.7602182394258672E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>42222</v>
       </c>
@@ -2359,8 +2446,11 @@
       <c r="W27">
         <v>1.2104715695364868E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>42109</v>
       </c>
@@ -2430,8 +2520,11 @@
       <c r="W28">
         <v>0.33758266435183909</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>42109</v>
       </c>
@@ -2501,8 +2594,11 @@
       <c r="W29">
         <v>3.5890822205253053E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>42109</v>
       </c>
@@ -2572,8 +2668,11 @@
       <c r="W30">
         <v>8.7391202347203864E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>42109</v>
       </c>
@@ -2643,8 +2742,11 @@
       <c r="W31">
         <v>3.576145899296141E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>42109</v>
       </c>
@@ -2714,8 +2816,11 @@
       <c r="W32">
         <v>5.7408412205219791E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>42109</v>
       </c>
@@ -2785,8 +2890,11 @@
       <c r="W33">
         <v>3.5273097066170933E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>42109</v>
       </c>
@@ -2856,8 +2964,11 @@
       <c r="W34">
         <v>1.4507684870760899E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>42109</v>
       </c>
@@ -2927,8 +3038,11 @@
       <c r="W35">
         <v>3.2730121778342176E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>42109</v>
       </c>
@@ -2998,8 +3112,11 @@
       <c r="W36">
         <v>1.7371334194068187E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>42109</v>
       </c>
@@ -3069,8 +3186,11 @@
       <c r="W37">
         <v>6.539021736521061E-3</v>
       </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>42109</v>
       </c>
@@ -3140,8 +3260,11 @@
       <c r="W38">
         <v>3.4608201122200782E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>42109</v>
       </c>
@@ -3211,8 +3334,11 @@
       <c r="W39">
         <v>1.4590761106039797E-3</v>
       </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>42109</v>
       </c>
@@ -3282,8 +3408,11 @@
       <c r="W40">
         <v>6.4629341545809722E-3</v>
       </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>42743</v>
       </c>
@@ -3354,10 +3483,13 @@
         <v>0.7372067375597412</v>
       </c>
       <c r="X41" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y41" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>42743</v>
       </c>
@@ -3428,10 +3560,13 @@
         <v>0.3334368195994068</v>
       </c>
       <c r="X42" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y42" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42743</v>
       </c>
@@ -3502,10 +3637,13 @@
         <v>3.4892100383338016E-2</v>
       </c>
       <c r="X43" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y43" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42743</v>
       </c>
@@ -3576,10 +3714,13 @@
         <v>4.3945270165990848E-2</v>
       </c>
       <c r="X44" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y44" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>42743</v>
       </c>
@@ -3650,10 +3791,13 @@
         <v>1.0404594789742616E-2</v>
       </c>
       <c r="X45" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y45" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>42743</v>
       </c>
@@ -3724,10 +3868,13 @@
         <v>2.6595582053983938E-3</v>
       </c>
       <c r="X46" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y46" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>42743</v>
       </c>
@@ -3798,10 +3945,13 @@
         <v>1.8701538611838944E-2</v>
       </c>
       <c r="X47" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y47" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>42743</v>
       </c>
@@ -3872,10 +4022,13 @@
         <v>1.8078414491013342E-2</v>
       </c>
       <c r="X48" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y48" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>42743</v>
       </c>
@@ -3946,10 +4099,13 @@
         <v>2.9301350634939112E-2</v>
       </c>
       <c r="X49" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y49" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>42743</v>
       </c>
@@ -4020,10 +4176,13 @@
         <v>1.9647459601046309E-2</v>
       </c>
       <c r="X50" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y50" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>42743</v>
       </c>
@@ -4094,10 +4253,13 @@
         <v>1.4795652009213204E-2</v>
       </c>
       <c r="X51" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y51" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>42743</v>
       </c>
@@ -4168,10 +4330,13 @@
         <v>3.9452331651423873E-2</v>
       </c>
       <c r="X52" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y52" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>42743</v>
       </c>
@@ -4242,10 +4407,13 @@
         <v>3.0922596265211658E-2</v>
       </c>
       <c r="X53" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y53" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>42963</v>
       </c>
@@ -4316,10 +4484,13 @@
         <v>0.35936110257340032</v>
       </c>
       <c r="X54" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y54" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>42963</v>
       </c>
@@ -4390,10 +4561,13 @@
         <v>3.6665467710530246E-2</v>
       </c>
       <c r="X55" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y55" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>42963</v>
       </c>
@@ -4464,10 +4638,13 @@
         <v>2.872373729530122E-2</v>
       </c>
       <c r="X56" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y56" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>42963</v>
       </c>
@@ -4538,10 +4715,13 @@
         <v>3.5180439273521234E-2</v>
       </c>
       <c r="X57" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y57" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>42963</v>
       </c>
@@ -4612,10 +4792,13 @@
         <v>2.4985671623482562E-2</v>
       </c>
       <c r="X58" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y58" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>42963</v>
       </c>
@@ -4686,10 +4869,13 @@
         <v>3.7340562520112752E-2</v>
       </c>
       <c r="X59" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y59" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>42963</v>
       </c>
@@ -4760,10 +4946,13 @@
         <v>4.739541876886179E-3</v>
       </c>
       <c r="X60" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y60" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>42963</v>
       </c>
@@ -4834,10 +5023,13 @@
         <v>1.6631654096574484E-2</v>
       </c>
       <c r="X61" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y61" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>42963</v>
       </c>
@@ -4908,10 +5100,13 @@
         <v>6.5489190252815285E-2</v>
       </c>
       <c r="X62" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y62" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>42963</v>
       </c>
@@ -4982,10 +5177,13 @@
         <v>2.7542899943947683E-2</v>
       </c>
       <c r="X63" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y63" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>42963</v>
       </c>
@@ -5056,10 +5254,13 @@
         <v>2.6184183088512709E-3</v>
       </c>
       <c r="X64" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y64" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>42963</v>
       </c>
@@ -5130,10 +5331,13 @@
         <v>1.1809772693272236E-2</v>
       </c>
       <c r="X65" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y65" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>42963</v>
       </c>
@@ -5204,10 +5408,13 @@
         <v>1.4975363926432522E-3</v>
       </c>
       <c r="X66" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y66" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>42079</v>
       </c>
@@ -5274,8 +5481,11 @@
       <c r="W67">
         <v>8.1771353568597355E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X67" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>42079</v>
       </c>
@@ -5342,8 +5552,11 @@
       <c r="W68">
         <v>0.13506536597363356</v>
       </c>
-    </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X68" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>42079</v>
       </c>
@@ -5410,8 +5623,11 @@
       <c r="W69">
         <v>6.3674069914939485E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X69" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>42079</v>
       </c>
@@ -5478,8 +5694,11 @@
       <c r="W70">
         <v>3.1157736720845968E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X70" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>42079</v>
       </c>
@@ -5546,8 +5765,11 @@
       <c r="W71">
         <v>1.1528543666970356E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X71" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>42079</v>
       </c>
@@ -5614,8 +5836,11 @@
       <c r="W72">
         <v>1.4465977415277644E-2</v>
       </c>
-    </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X72" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>42079</v>
       </c>
@@ -5682,8 +5907,11 @@
       <c r="W73">
         <v>6.3064270844627304E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X73" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>42079</v>
       </c>
@@ -5750,8 +5978,11 @@
       <c r="W74">
         <v>8.9413761321149893E-2</v>
       </c>
-    </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X74" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>42079</v>
       </c>
@@ -5818,8 +6049,11 @@
       <c r="W75">
         <v>2.3538062126835155E-2</v>
       </c>
-    </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X75" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="76" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>42079</v>
       </c>
@@ -5886,8 +6120,11 @@
       <c r="W76">
         <v>1.6585813546941559E-2</v>
       </c>
-    </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X76" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>42079</v>
       </c>
@@ -5954,8 +6191,11 @@
       <c r="W77">
         <v>1.2386422264479217E-2</v>
       </c>
-    </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X77" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>42079</v>
       </c>
@@ -6022,8 +6262,11 @@
       <c r="W78">
         <v>1.8650854691572495E-2</v>
       </c>
-    </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X78" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>42476</v>
       </c>
@@ -6093,8 +6336,11 @@
       <c r="W79">
         <v>0.22903858570787416</v>
       </c>
-    </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X79" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>42476</v>
       </c>
@@ -6164,8 +6410,11 @@
       <c r="W80">
         <v>2.2191758252145848E-2</v>
       </c>
-    </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X80" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>42476</v>
       </c>
@@ -6235,8 +6484,11 @@
       <c r="W81">
         <v>0.11670467399009229</v>
       </c>
-    </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X81" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>42476</v>
       </c>
@@ -6306,8 +6558,11 @@
       <c r="W82">
         <v>5.1296130330414698E-2</v>
       </c>
-    </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X82" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>42476</v>
       </c>
@@ -6377,8 +6632,11 @@
       <c r="W83">
         <v>2.182466670607057E-2</v>
       </c>
-    </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X83" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>42476</v>
       </c>
@@ -6448,8 +6706,11 @@
       <c r="W84">
         <v>1.4474269306707374E-2</v>
       </c>
-    </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X84" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>42476</v>
       </c>
@@ -6519,8 +6780,11 @@
       <c r="W85">
         <v>1.9529701577678939E-2</v>
       </c>
-    </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X85" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>42476</v>
       </c>
@@ -6590,8 +6854,11 @@
       <c r="W86">
         <v>2.3335886396181491E-2</v>
       </c>
-    </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X86" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>42476</v>
       </c>
@@ -6661,8 +6928,11 @@
       <c r="W87">
         <v>3.8510965890794967E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X87" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>42476</v>
       </c>
@@ -6732,8 +7002,11 @@
       <c r="W88">
         <v>2.1543166908768192E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X88" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>42476</v>
       </c>
@@ -6803,8 +7076,11 @@
       <c r="W89">
         <v>1.0022796871960326E-2</v>
       </c>
-    </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X89" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>42476</v>
       </c>
@@ -6874,8 +7150,11 @@
       <c r="W90">
         <v>3.261772779350709E-3</v>
       </c>
-    </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X90" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>42476</v>
       </c>
@@ -6945,8 +7224,11 @@
       <c r="W91">
         <v>1.0997334646163464E-2</v>
       </c>
-    </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X91" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>42857</v>
       </c>
@@ -7016,8 +7298,11 @@
       <c r="W92">
         <v>3.6677382511260674E-2</v>
       </c>
-    </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X92" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>42857</v>
       </c>
@@ -7087,8 +7372,11 @@
       <c r="W93">
         <v>0.15360986890120287</v>
       </c>
-    </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X93" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>42857</v>
       </c>
@@ -7158,8 +7446,11 @@
       <c r="W94">
         <v>2.1614561458425479E-2</v>
       </c>
-    </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X94" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>42857</v>
       </c>
@@ -7229,8 +7520,11 @@
       <c r="W95">
         <v>4.2275251136423851E-2</v>
       </c>
-    </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X95" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>42857</v>
       </c>
@@ -7300,8 +7594,11 @@
       <c r="W96">
         <v>2.2606633908916922E-2</v>
       </c>
-    </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X96" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="97" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>42857</v>
       </c>
@@ -7371,8 +7668,11 @@
       <c r="W97">
         <v>2.2944269004881983E-2</v>
       </c>
-    </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X97" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="98" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>42857</v>
       </c>
@@ -7442,8 +7742,11 @@
       <c r="W98">
         <v>3.6299356223706405E-2</v>
       </c>
-    </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X98" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="99" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>42857</v>
       </c>
@@ -7513,8 +7816,11 @@
       <c r="W99">
         <v>9.8909177337326813E-3</v>
       </c>
-    </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X99" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="100" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>42857</v>
       </c>
@@ -7584,8 +7890,11 @@
       <c r="W100">
         <v>5.4453687950713299E-3</v>
       </c>
-    </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X100" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="101" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>42857</v>
       </c>
@@ -7655,8 +7964,11 @@
       <c r="W101">
         <v>2.0895735949445132E-2</v>
       </c>
-    </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X101" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>42857</v>
       </c>
@@ -7726,8 +8038,11 @@
       <c r="W102">
         <v>1.8899181362303005E-2</v>
       </c>
-    </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X102" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="103" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>42857</v>
       </c>
@@ -7797,8 +8112,11 @@
       <c r="W103">
         <v>9.8995820444115531E-3</v>
       </c>
-    </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X103" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="104" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>43207</v>
       </c>
@@ -7869,10 +8187,13 @@
         <v>0.1127110563304569</v>
       </c>
       <c r="X104" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y104" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>43207</v>
       </c>
@@ -7943,10 +8264,13 @@
         <v>6.1534736729600775E-2</v>
       </c>
       <c r="X105" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y105" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>43207</v>
       </c>
@@ -8017,10 +8341,13 @@
         <v>4.7777019034894362E-2</v>
       </c>
       <c r="X106" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y106" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>43207</v>
       </c>
@@ -8091,10 +8418,13 @@
         <v>1.1575466112225901E-3</v>
       </c>
       <c r="X107" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y107" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>43207</v>
       </c>
@@ -8165,10 +8495,13 @@
         <v>1.2940827117340971E-2</v>
       </c>
       <c r="X108" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y108" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>43207</v>
       </c>
@@ -8239,10 +8572,13 @@
         <v>2.1269562694013585E-2</v>
       </c>
       <c r="X109" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y109" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>43207</v>
       </c>
@@ -8313,10 +8649,13 @@
         <v>3.6384485859625629E-2</v>
       </c>
       <c r="X110" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y110" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>43207</v>
       </c>
@@ -8387,10 +8726,13 @@
         <v>4.5062648547826347E-3</v>
       </c>
       <c r="X111" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y111" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>43207</v>
       </c>
@@ -8461,10 +8803,13 @@
         <v>3.8446399190032282E-4</v>
       </c>
       <c r="X112" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y112" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>43207</v>
       </c>
@@ -8535,10 +8880,13 @@
         <v>1.381393360695808E-2</v>
       </c>
       <c r="X113" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y113" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>43207</v>
       </c>
@@ -8608,8 +8956,11 @@
       <c r="W114">
         <v>3.8252878724317698E-3</v>
       </c>
-    </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X114" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="115" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>43207</v>
       </c>
@@ -8679,8 +9030,11 @@
       <c r="W115">
         <v>4.9226714259983278E-4</v>
       </c>
-    </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X115" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="116" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>43207</v>
       </c>
@@ -8750,8 +9104,11 @@
       <c r="W116">
         <v>4.5870582356601303E-4</v>
       </c>
-    </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X116" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="117" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>43207</v>
       </c>
@@ -8821,8 +9178,11 @@
       <c r="W117">
         <v>9.4892473141659588E-4</v>
       </c>
-    </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X117" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="118" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>43207</v>
       </c>
@@ -8892,8 +9252,11 @@
       <c r="W118">
         <v>9.5472430303452961E-3</v>
       </c>
-    </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X118" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="119" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>43207</v>
       </c>
@@ -8963,8 +9326,11 @@
       <c r="W119">
         <v>5.4696043783697768E-3</v>
       </c>
-    </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X119" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="120" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>43207</v>
       </c>
@@ -9034,8 +9400,11 @@
       <c r="W120">
         <v>3.6672581990071951E-2</v>
       </c>
-    </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X120" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="121" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>43207</v>
       </c>
@@ -9105,8 +9474,11 @@
       <c r="W121">
         <v>3.2020337373225333E-3</v>
       </c>
-    </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X121" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="122" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>43207</v>
       </c>
@@ -9176,8 +9548,11 @@
       <c r="W122">
         <v>6.1245119125506635E-3</v>
       </c>
-    </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X122" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="123" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>43207</v>
       </c>
@@ -9247,8 +9622,11 @@
       <c r="W123">
         <v>3.8523774962330893E-4</v>
       </c>
-    </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X123" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="124" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>43224</v>
       </c>
@@ -9318,8 +9696,11 @@
       <c r="W124">
         <v>0.11722899193319915</v>
       </c>
-    </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X124" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="125" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>43224</v>
       </c>
@@ -9389,8 +9770,11 @@
       <c r="W125">
         <v>7.8420639162332158E-3</v>
       </c>
-    </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X125" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="126" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>43224</v>
       </c>
@@ -9460,8 +9844,11 @@
       <c r="W126">
         <v>1.5177154447999476E-2</v>
       </c>
-    </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X126" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="127" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>43224</v>
       </c>
@@ -9531,8 +9918,11 @@
       <c r="W127">
         <v>2.4372876775915819E-2</v>
       </c>
-    </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X127" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="128" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>43224</v>
       </c>
@@ -9602,8 +9992,11 @@
       <c r="W128">
         <v>1.5554613725222237E-2</v>
       </c>
-    </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X128" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="129" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>43224</v>
       </c>
@@ -9673,8 +10066,11 @@
       <c r="W129">
         <v>3.7187868102742292E-3</v>
       </c>
-    </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X129" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="130" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>43224</v>
       </c>
@@ -9744,8 +10140,11 @@
       <c r="W130">
         <v>1.4926609089124779E-2</v>
       </c>
-    </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X130" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="131" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>43224</v>
       </c>
@@ -9815,8 +10214,11 @@
       <c r="W131">
         <v>4.5091030354387556E-3</v>
       </c>
-    </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X131" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="132" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>43594</v>
       </c>
@@ -9886,8 +10288,11 @@
       <c r="W132">
         <v>9.2706791696502908E-3</v>
       </c>
-    </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X132" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="133" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>43594</v>
       </c>
@@ -9957,8 +10362,11 @@
       <c r="W133">
         <v>3.662681341900545E-2</v>
       </c>
-    </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X133" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="134" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>43594</v>
       </c>
@@ -10028,8 +10436,11 @@
       <c r="W134">
         <v>1.5559139679553038E-2</v>
       </c>
-    </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X134" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="135" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>43594</v>
       </c>
@@ -10099,8 +10510,11 @@
       <c r="W135">
         <v>2.8673114886499377E-2</v>
       </c>
-    </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X135" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="136" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>43594</v>
       </c>
@@ -10170,8 +10584,11 @@
       <c r="W136">
         <v>7.7300940989731186E-3</v>
       </c>
-    </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X136" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="137" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>43594</v>
       </c>
@@ -10241,8 +10658,11 @@
       <c r="W137">
         <v>2.4922977192912486E-3</v>
       </c>
-    </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X137" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="138" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>43594</v>
       </c>
@@ -10312,8 +10732,11 @@
       <c r="W138">
         <v>1.425741353787598E-2</v>
       </c>
-    </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X138" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="139" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>43224</v>
       </c>
@@ -10383,8 +10806,11 @@
       <c r="W139">
         <v>9.0826062884745609E-2</v>
       </c>
-    </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X139" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="140" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>43224</v>
       </c>
@@ -10454,8 +10880,11 @@
       <c r="W140">
         <v>1.0694731754243025E-2</v>
       </c>
-    </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X140" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="141" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>43224</v>
       </c>
@@ -10525,8 +10954,11 @@
       <c r="W141">
         <v>5.7609896285922488E-3</v>
       </c>
-    </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X141" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="142" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>43224</v>
       </c>
@@ -10596,8 +11028,11 @@
       <c r="W142">
         <v>1.8931671433800354E-2</v>
       </c>
-    </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X142" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="143" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>43224</v>
       </c>
@@ -10667,8 +11102,11 @@
       <c r="W143">
         <v>2.0036809728549952E-3</v>
       </c>
-    </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X143" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="144" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>43224</v>
       </c>
@@ -10738,8 +11176,11 @@
       <c r="W144">
         <v>5.8138452108270301E-3</v>
       </c>
-    </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X144" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="145" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>43224</v>
       </c>
@@ -10809,8 +11250,11 @@
       <c r="W145">
         <v>8.3840204543507227E-3</v>
       </c>
-    </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X145" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="146" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>43224</v>
       </c>
@@ -10880,8 +11324,11 @@
       <c r="W146">
         <v>7.2128334198104313E-3</v>
       </c>
-    </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X146" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="147" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>43594</v>
       </c>
@@ -10951,8 +11398,11 @@
       <c r="W147">
         <v>1.5163298858960004E-2</v>
       </c>
-    </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X147" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="148" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>43594</v>
       </c>
@@ -11022,8 +11472,11 @@
       <c r="W148">
         <v>4.1264583145844101E-3</v>
       </c>
-    </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X148" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="149" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>43594</v>
       </c>
@@ -11093,8 +11546,11 @@
       <c r="W149">
         <v>7.6739288312050293E-3</v>
       </c>
-    </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X149" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="150" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>43594</v>
       </c>
@@ -11164,8 +11620,11 @@
       <c r="W150">
         <v>1.6415710865679816E-2</v>
       </c>
-    </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X150" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="151" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>43594</v>
       </c>
@@ -11235,8 +11694,11 @@
       <c r="W151">
         <v>7.4425331165766523E-4</v>
       </c>
-    </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X151" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="152" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>43594</v>
       </c>
@@ -11306,8 +11768,11 @@
       <c r="W152">
         <v>6.9056502303580566E-3</v>
       </c>
-    </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X152" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="153" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>43594</v>
       </c>
@@ -11376,6 +11841,9 @@
       </c>
       <c r="W153">
         <v>6.9428494621533729E-3</v>
+      </c>
+      <c r="X153" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>